<commit_message>
colour changes to backlog
</commit_message>
<xml_diff>
--- a/doc/Product-backlog.xlsx
+++ b/doc/Product-backlog.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Effort</t>
   </si>
@@ -80,13 +80,28 @@
   </si>
   <si>
     <t>Design the GUI looks</t>
+  </si>
+  <si>
+    <t>Ha en search, och så ligger &lt; inom den sprinten?</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Frontend: Advanced search</t>
+  </si>
+  <si>
+    <t>Backend: advnced Search</t>
+  </si>
+  <si>
+    <t>Ha ett backlig item för en sak, och i sprinten dela upp i backend och frontend?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,6 +120,19 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -130,7 +158,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -142,6 +170,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -178,13 +208,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D20" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:D20"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E22" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:E22"/>
+  <tableColumns count="5">
     <tableColumn id="5" name="Id" dataDxfId="0"/>
     <tableColumn id="1" name="Features"/>
     <tableColumn id="3" name="Value"/>
     <tableColumn id="4" name="Effort"/>
+    <tableColumn id="2" name="Column1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -477,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,7 +524,7 @@
     <col min="6" max="6" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -506,8 +537,11 @@
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -521,7 +555,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -535,7 +569,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -549,7 +583,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -563,11 +597,11 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C6">
@@ -577,11 +611,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C7">
@@ -591,11 +625,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C8">
@@ -605,11 +639,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C9">
@@ -619,11 +653,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C10">
@@ -633,11 +667,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C11">
@@ -647,99 +681,93 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" s="6" t="s">
         <v>6</v>
-      </c>
-      <c r="C12">
-        <v>6</v>
-      </c>
-      <c r="D12">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>5</v>
       </c>
       <c r="C13">
         <v>6</v>
       </c>
       <c r="D13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
+        <v>8</v>
+      </c>
+      <c r="E13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14">
+        <v>6</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>12</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <v>6</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B16" t="s">
         <v>7</v>
       </c>
-      <c r="C14">
-        <v>2</v>
-      </c>
-      <c r="D14">
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
         <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15">
-        <v>5</v>
-      </c>
-      <c r="D15">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16">
-        <v>3</v>
-      </c>
-      <c r="D16">
-        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>10</v>
+        <v>14</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="C17">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D17">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="C18">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D18">
         <v>4</v>
@@ -747,23 +775,51 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19">
+        <v>6</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>17</v>
+      </c>
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20">
+        <v>5</v>
+      </c>
+      <c r="D20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B21" t="s">
         <v>21</v>
       </c>
-      <c r="C19">
+      <c r="C21">
         <v>5</v>
       </c>
-      <c r="D19">
+      <c r="D21">
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C20" s="4"/>
-      <c r="D20" s="4" t="str">
-        <f>("Sum: "&amp;SUBTOTAL(109,D2:D19))</f>
-        <v>Sum: 81</v>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C22" s="4"/>
+      <c r="D22" s="4" t="str">
+        <f>("Sum: "&amp;SUBTOTAL(109,D2:D21))</f>
+        <v>Sum: 83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>